<commit_message>
Remove cyano from input data requirements
Cyanobacteria is predicted by the model, but it is not actually required as an input. The input format can therefore be simplified.
</commit_message>
<xml_diff>
--- a/app/chemistry_data/seasonal_obs_vanemfjorden.xlsx
+++ b/app/chemistry_data/seasonal_obs_vanemfjorden.xlsx
@@ -5,20 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JES\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\James_Work\Staff\Leah_JB\WateXr\watexr_voila_app\app\chemistry_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A9F214E-502D-42BD-9480-1B3032FE603D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E97FC49-3B9B-4A7E-A4D3-CCE45947EDCA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{A865B059-BBFE-4C6B-B3E9-E2D8DA065CB3}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="1" xr2:uid="{A865B059-BBFE-4C6B-B3E9-E2D8DA065CB3}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="2" r:id="rId1"/>
     <sheet name="data" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">data!$A$1:$E$41</definedName>
-    <definedName name="seasonal_obs_no_trans_1980_2019" localSheetId="1">data!$A$1:$E$41</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">data!$A$1:$D$41</definedName>
+    <definedName name="seasonal_obs_no_trans_1980_2019" localSheetId="1">data!$A$1:$D$41</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>year</t>
   </si>
@@ -64,9 +64,6 @@
   </si>
   <si>
     <t>mean_colour_mgPtpl</t>
-  </si>
-  <si>
-    <t>max_cyano_mm3pl</t>
   </si>
 </sst>
 </file>
@@ -321,28 +318,6 @@
           <a:r>
             <a:rPr lang="en-GB" sz="1100" baseline="0"/>
             <a:t> colour (mgPt/l)</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
-            <a:t> - </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" b="1" baseline="0"/>
-            <a:t>max_cyano</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
-            <a:t>	</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" i="1" baseline="0"/>
-            <a:t>Maximum</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
-            <a:t> cyanobacteria (mm3/l)</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -754,7 +729,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D22D3743-475C-476A-860D-8BD32DD142C0}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
@@ -767,11 +742,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF0A4113-C129-4948-A177-EB5CB1A86A5A}">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -780,10 +755,9 @@
     <col min="2" max="2" width="15.265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -796,11 +770,8 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1980</v>
       </c>
@@ -811,7 +782,7 @@
         <v>16.0801298702727</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>1981</v>
       </c>
@@ -822,7 +793,7 @@
         <v>8.3312500000000007</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>1982</v>
       </c>
@@ -836,7 +807,7 @@
         <v>26.6666666666666</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>1983</v>
       </c>
@@ -850,7 +821,7 @@
         <v>17.625</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>1984</v>
       </c>
@@ -861,7 +832,7 @@
         <v>11.09</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>1985</v>
       </c>
@@ -875,7 +846,7 @@
         <v>34.404761904285699</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>1986</v>
       </c>
@@ -889,7 +860,7 @@
         <v>27.472222223333301</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>1987</v>
       </c>
@@ -903,7 +874,7 @@
         <v>29.027777778333299</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>1988</v>
       </c>
@@ -917,7 +888,7 @@
         <v>32.277777776666603</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>1989</v>
       </c>
@@ -931,7 +902,7 @@
         <v>23.857142857142801</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>1990</v>
       </c>
@@ -945,7 +916,7 @@
         <v>19.857142857142801</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>1991</v>
       </c>
@@ -959,7 +930,7 @@
         <v>20.625</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>1992</v>
       </c>
@@ -973,7 +944,7 @@
         <v>21.285714285714199</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>1993</v>
       </c>
@@ -987,7 +958,7 @@
         <v>24.428571428571399</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>1994</v>
       </c>
@@ -1001,7 +972,7 @@
         <v>27.714285714285701</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>1995</v>
       </c>
@@ -1015,7 +986,7 @@
         <v>25.8333333333333</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>1996</v>
       </c>
@@ -1028,11 +999,8 @@
       <c r="D18">
         <v>17.6666666666666</v>
       </c>
-      <c r="E18">
-        <v>4.8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>1997</v>
       </c>
@@ -1045,11 +1013,8 @@
       <c r="D19">
         <v>19</v>
       </c>
-      <c r="E19">
-        <v>2.82</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>1998</v>
       </c>
@@ -1059,22 +1024,16 @@
       <c r="C20">
         <v>21.099999999999898</v>
       </c>
-      <c r="E20">
-        <v>2.2799999999999998</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>1999</v>
       </c>
       <c r="D21">
         <v>50.423076923076898</v>
       </c>
-      <c r="E21">
-        <v>5.96</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>2000</v>
       </c>
@@ -1087,11 +1046,8 @@
       <c r="D22">
         <v>42.56</v>
       </c>
-      <c r="E22">
-        <v>4.67</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>2001</v>
       </c>
@@ -1104,11 +1060,8 @@
       <c r="D23">
         <v>68.423076923076906</v>
       </c>
-      <c r="E23">
-        <v>0.57999999999999996</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>2002</v>
       </c>
@@ -1121,11 +1074,8 @@
       <c r="D24">
         <v>54.576923076923002</v>
       </c>
-      <c r="E24">
-        <v>0.98199999999999998</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>2003</v>
       </c>
@@ -1138,11 +1088,8 @@
       <c r="D25">
         <v>42.875</v>
       </c>
-      <c r="E25">
-        <v>1.2909999999999999</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>2004</v>
       </c>
@@ -1155,11 +1102,8 @@
       <c r="D26">
         <v>38.6666666666666</v>
       </c>
-      <c r="E26">
-        <v>5.26</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>2005</v>
       </c>
@@ -1172,11 +1116,8 @@
       <c r="D27">
         <v>46.5</v>
       </c>
-      <c r="E27">
-        <v>3.06259999999999</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>2006</v>
       </c>
@@ -1189,11 +1130,8 @@
       <c r="D28">
         <v>48.3333333333333</v>
       </c>
-      <c r="E28">
-        <v>4.5602</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>2007</v>
       </c>
@@ -1206,11 +1144,8 @@
       <c r="D29">
         <v>64.6666666666666</v>
       </c>
-      <c r="E29">
-        <v>3.5880000000000001</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30">
         <v>2008</v>
       </c>
@@ -1223,11 +1158,8 @@
       <c r="D30">
         <v>69</v>
       </c>
-      <c r="E30">
-        <v>0.73899999999999999</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31">
         <v>2009</v>
       </c>
@@ -1240,11 +1172,8 @@
       <c r="D31">
         <v>58.285714285714199</v>
       </c>
-      <c r="E31">
-        <v>1.5860000000000001</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>2010</v>
       </c>
@@ -1257,11 +1186,8 @@
       <c r="D32">
         <v>61.714285714285701</v>
       </c>
-      <c r="E32">
-        <v>0.224</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33">
         <v>2011</v>
       </c>
@@ -1274,11 +1200,8 @@
       <c r="D33">
         <v>72.8888888888888</v>
       </c>
-      <c r="E33">
-        <v>7.9000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34">
         <v>2012</v>
       </c>
@@ -1291,11 +1214,8 @@
       <c r="D34">
         <v>64.153846153846104</v>
       </c>
-      <c r="E34">
-        <v>0.21099999999999999</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35">
         <v>2013</v>
       </c>
@@ -1308,11 +1228,8 @@
       <c r="D35">
         <v>60.223076923076903</v>
       </c>
-      <c r="E35">
-        <v>0.53400000000000003</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36">
         <v>2014</v>
       </c>
@@ -1325,11 +1242,8 @@
       <c r="D36">
         <v>41.863636363636303</v>
       </c>
-      <c r="E36">
-        <v>0.28299999999999997</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37">
         <v>2015</v>
       </c>
@@ -1342,11 +1256,8 @@
       <c r="D37">
         <v>52.8333333333333</v>
       </c>
-      <c r="E37">
-        <v>0.23300000000000001</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38">
         <v>2016</v>
       </c>
@@ -1359,11 +1270,8 @@
       <c r="D38">
         <v>52</v>
       </c>
-      <c r="E38">
-        <v>0.16600000000000001</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39">
         <v>2017</v>
       </c>
@@ -1376,11 +1284,8 @@
       <c r="D39">
         <v>42</v>
       </c>
-      <c r="E39">
-        <v>0.25800000000000001</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40">
         <v>2018</v>
       </c>
@@ -1393,11 +1298,8 @@
       <c r="D40">
         <v>36.3333333333333</v>
       </c>
-      <c r="E40">
-        <v>0.61399999999999999</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41">
         <v>2019</v>
       </c>
@@ -1410,12 +1312,9 @@
       <c r="D41">
         <v>47</v>
       </c>
-      <c r="E41">
-        <v>0.59199999999999997</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E41" xr:uid="{3528EE9F-E04B-4056-8A0A-FADA771746D3}"/>
+  <autoFilter ref="A1:D41" xr:uid="{3528EE9F-E04B-4056-8A0A-FADA771746D3}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix units in chem file
</commit_message>
<xml_diff>
--- a/app/chemistry_data/seasonal_obs_vanemfjorden.xlsx
+++ b/app/chemistry_data/seasonal_obs_vanemfjorden.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\James_Work\Staff\Leah_JB\WateXr\watexr_voila_app\app\chemistry_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E97FC49-3B9B-4A7E-A4D3-CCE45947EDCA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B83162F-3E0C-45B6-BE74-B2F98127044F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="1" xr2:uid="{A865B059-BBFE-4C6B-B3E9-E2D8DA065CB3}"/>
+    <workbookView xWindow="14385" yWindow="0" windowWidth="14415" windowHeight="15600" activeTab="1" xr2:uid="{A865B059-BBFE-4C6B-B3E9-E2D8DA065CB3}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="2" r:id="rId1"/>
@@ -57,13 +57,13 @@
     <t>year</t>
   </si>
   <si>
-    <t>mean_tp_mgpl</t>
-  </si>
-  <si>
     <t>mean_chla_mgpl</t>
   </si>
   <si>
     <t>mean_colour_mgPtpl</t>
+  </si>
+  <si>
+    <t>mean_tp_ugpl</t>
   </si>
 </sst>
 </file>
@@ -746,7 +746,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -762,13 +762,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Added observations for 2020
</commit_message>
<xml_diff>
--- a/app/chemistry_data/seasonal_obs_vanemfjorden.xlsx
+++ b/app/chemistry_data/seasonal_obs_vanemfjorden.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\James_Work\Staff\Leah_JB\WateXr\watexr_voila_app\app\chemistry_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\GitHub\watexr_voila_app\app\chemistry_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1176D1EB-8B90-4645-B6C5-7BB452F7A34E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E94FFDBF-B2D8-41ED-8498-D0ECBF27A452}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14385" yWindow="0" windowWidth="14415" windowHeight="15600" activeTab="1" xr2:uid="{A865B059-BBFE-4C6B-B3E9-E2D8DA065CB3}"/>
+    <workbookView xWindow="795" yWindow="420" windowWidth="21600" windowHeight="11325" activeTab="1" xr2:uid="{A865B059-BBFE-4C6B-B3E9-E2D8DA065CB3}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="2" r:id="rId1"/>
@@ -735,7 +735,7 @@
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -744,22 +744,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF0A4113-C129-4948-A177-EB5CB1A86A5A}">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.46484375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.3984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -773,7 +773,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1980</v>
       </c>
@@ -784,7 +784,7 @@
         <v>16.0801298702727</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1981</v>
       </c>
@@ -795,7 +795,7 @@
         <v>8.3312500000000007</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1982</v>
       </c>
@@ -809,7 +809,7 @@
         <v>26.6666666666666</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1983</v>
       </c>
@@ -823,7 +823,7 @@
         <v>17.625</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1984</v>
       </c>
@@ -834,7 +834,7 @@
         <v>11.09</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1985</v>
       </c>
@@ -848,7 +848,7 @@
         <v>34.404761904285699</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1986</v>
       </c>
@@ -862,7 +862,7 @@
         <v>27.472222223333301</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1987</v>
       </c>
@@ -876,7 +876,7 @@
         <v>29.027777778333299</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1988</v>
       </c>
@@ -890,7 +890,7 @@
         <v>32.277777776666603</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1989</v>
       </c>
@@ -904,7 +904,7 @@
         <v>23.857142857142801</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1990</v>
       </c>
@@ -918,7 +918,7 @@
         <v>19.857142857142801</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1991</v>
       </c>
@@ -932,7 +932,7 @@
         <v>20.625</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1992</v>
       </c>
@@ -946,7 +946,7 @@
         <v>21.285714285714199</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1993</v>
       </c>
@@ -960,7 +960,7 @@
         <v>24.428571428571399</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1994</v>
       </c>
@@ -974,7 +974,7 @@
         <v>27.714285714285701</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1995</v>
       </c>
@@ -988,7 +988,7 @@
         <v>25.8333333333333</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1996</v>
       </c>
@@ -1002,7 +1002,7 @@
         <v>17.6666666666666</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1997</v>
       </c>
@@ -1016,7 +1016,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1998</v>
       </c>
@@ -1027,7 +1027,7 @@
         <v>21.099999999999898</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1999</v>
       </c>
@@ -1035,7 +1035,7 @@
         <v>50.423076923076898</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2000</v>
       </c>
@@ -1049,7 +1049,7 @@
         <v>42.56</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2001</v>
       </c>
@@ -1063,7 +1063,7 @@
         <v>68.423076923076906</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2002</v>
       </c>
@@ -1077,7 +1077,7 @@
         <v>54.576923076923002</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2003</v>
       </c>
@@ -1091,7 +1091,7 @@
         <v>42.875</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2004</v>
       </c>
@@ -1105,7 +1105,7 @@
         <v>38.6666666666666</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2005</v>
       </c>
@@ -1119,7 +1119,7 @@
         <v>46.5</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2006</v>
       </c>
@@ -1133,7 +1133,7 @@
         <v>48.3333333333333</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2007</v>
       </c>
@@ -1147,7 +1147,7 @@
         <v>64.6666666666666</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2008</v>
       </c>
@@ -1161,7 +1161,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2009</v>
       </c>
@@ -1175,7 +1175,7 @@
         <v>58.285714285714199</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2010</v>
       </c>
@@ -1189,7 +1189,7 @@
         <v>61.714285714285701</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2011</v>
       </c>
@@ -1203,7 +1203,7 @@
         <v>72.8888888888888</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2012</v>
       </c>
@@ -1217,7 +1217,7 @@
         <v>64.153846153846104</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2013</v>
       </c>
@@ -1231,7 +1231,7 @@
         <v>60.223076923076903</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2014</v>
       </c>
@@ -1245,7 +1245,7 @@
         <v>41.863636363636303</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2015</v>
       </c>
@@ -1259,7 +1259,7 @@
         <v>52.8333333333333</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2016</v>
       </c>
@@ -1273,7 +1273,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2017</v>
       </c>
@@ -1287,7 +1287,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2018</v>
       </c>
@@ -1301,7 +1301,7 @@
         <v>36.3333333333333</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2019</v>
       </c>
@@ -1313,6 +1313,20 @@
       </c>
       <c r="D41" s="3">
         <v>47</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>2020</v>
+      </c>
+      <c r="B42" s="3">
+        <v>31.83</v>
+      </c>
+      <c r="C42" s="3">
+        <v>11.775</v>
+      </c>
+      <c r="D42" s="3">
+        <v>49.33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>